<commit_message>
all data complete and overleaf updated
</commit_message>
<xml_diff>
--- a/comment_Analysis/stack_overflow_analysis.xlsx
+++ b/comment_Analysis/stack_overflow_analysis.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloehebert/Documents/csc400/issuecomments_analysis/comment_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\issuecomments_analysis\comment_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1664EBF5-C7C0-4B84-9D62-37E1B53BD832}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="500" windowWidth="24560" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="3900" yWindow="600" windowWidth="28320" windowHeight="21000" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stack_baseline" sheetId="1" r:id="rId1"/>
     <sheet name="AWS" sheetId="2" r:id="rId2"/>
+    <sheet name="Google" sheetId="3" r:id="rId3"/>
+    <sheet name="Microsoft" sheetId="4" r:id="rId4"/>
+    <sheet name="IBM" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="20">
   <si>
     <t>Positive</t>
   </si>
@@ -62,12 +72,36 @@
   <si>
     <t>Macro avg</t>
   </si>
+  <si>
+    <t>GoogleMismatch</t>
+  </si>
+  <si>
+    <t>BaseLine</t>
+  </si>
+  <si>
+    <t>True Positive</t>
+  </si>
+  <si>
+    <t>False Positive</t>
+  </si>
+  <si>
+    <t>Cohen Kappa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mismatch</t>
+  </si>
+  <si>
+    <t>Negitive</t>
+  </si>
+  <si>
+    <t>mismatch</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +115,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,14 +143,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -119,12 +159,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -167,7 +210,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -241,17 +283,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1527.0</c:v>
+                  <c:v>1527</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1202.0</c:v>
+                  <c:v>1202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1694.0</c:v>
+                  <c:v>1694</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C14-434A-AEE1-7772DA3A3AB8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -419,7 +466,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -458,7 +505,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -532,17 +578,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1540.0</c:v>
+                  <c:v>1540</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1425.0</c:v>
+                  <c:v>1425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1561.0</c:v>
+                  <c:v>1561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3261-43AE-9CDA-C5B16BDF1132}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -709,6 +760,917 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Google Breakdown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Google!$A$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Positive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Google!$A$2:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1765</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-889B-40AB-84E1-2B2013A9877B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1764894671"/>
+        <c:axId val="1728240431"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1764894671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1728240431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1728240431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1764894671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Microsoft</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> breakdown</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Microsoft!$A$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Positive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Microsoft!$A$2:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1480</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-180B-4FED-8E46-FC6D1554166B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1821637903"/>
+        <c:axId val="1776639711"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1821637903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1776639711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1776639711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821637903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Watson Breakdown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>IBM!$A$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Positive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Negitive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>IBM!$A$2:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1822</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>809</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1738</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D99A-444A-A504-C7F0DDC47CDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1822534463"/>
+        <c:axId val="1823571967"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1822534463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1823571967"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1823571967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1822534463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -789,6 +1751,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1293,6 +2375,1515 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1812,7 +4403,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1847,7 +4444,136 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B28C0F4-ADA8-4FBE-A51D-ED16B837D09B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9C2391-3BFA-42EE-BA1F-5093EB6505AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D935E60-029E-4BEA-8273-EB965E2DE6D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2127,16 +4853,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2147,7 +4873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1527</v>
       </c>
@@ -2165,16 +4891,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2185,7 +4911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1540</v>
       </c>
@@ -2196,7 +4922,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2204,7 +4930,7 @@
         <v>0.31727</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2224,7 +4950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2247,7 +4973,7 @@
         <v>0.48954128440366973</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -2270,7 +4996,7 @@
         <v>0.32656514382402707</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2293,7 +5019,7 @@
         <v>0.53144311159578328</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2308,7 +5034,7 @@
         <v>0.53832226916113457</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2329,4 +5055,630 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EDCCC2-3756-40B6-90F4-186042FD4ADE}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1327</v>
+      </c>
+      <c r="B2">
+        <v>1331</v>
+      </c>
+      <c r="C2">
+        <v>1765</v>
+      </c>
+      <c r="D2">
+        <v>1312</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2">
+        <v>1527</v>
+      </c>
+      <c r="I2">
+        <v>1202</v>
+      </c>
+      <c r="J2">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <f>A2-C7</f>
+        <v>1170</v>
+      </c>
+      <c r="C7">
+        <v>157</v>
+      </c>
+      <c r="D7" s="1">
+        <f>B7/(B7+C7)</f>
+        <v>0.88168801808590802</v>
+      </c>
+      <c r="E7" s="1">
+        <f>B7/H2</f>
+        <v>0.76620825147347738</v>
+      </c>
+      <c r="F7" s="1">
+        <f>2*D7*E7/(D7+E7)</f>
+        <v>0.8199018920812895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>C2-C8</f>
+        <v>1062</v>
+      </c>
+      <c r="C8">
+        <v>703</v>
+      </c>
+      <c r="D8" s="1">
+        <f>B8/(B8+C8)</f>
+        <v>0.60169971671388101</v>
+      </c>
+      <c r="E8" s="1">
+        <f>B8/I2</f>
+        <v>0.88352745424292845</v>
+      </c>
+      <c r="F8" s="1">
+        <f>2*D8*E8/(D8+E8)</f>
+        <v>0.71587462082912035</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f>B2-C9</f>
+        <v>879</v>
+      </c>
+      <c r="C9">
+        <v>452</v>
+      </c>
+      <c r="D9" s="1">
+        <f>B9/(B9+C9)</f>
+        <v>0.66040570999248682</v>
+      </c>
+      <c r="E9" s="1">
+        <f>B9/J2</f>
+        <v>0.51889020070838254</v>
+      </c>
+      <c r="F9" s="1">
+        <f>2*D9*E9/(D9+E9)</f>
+        <v>0.58115702479338838</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
+        <f>(B7+B8+B9)/(B7+B8+B9+C7+C8+C9)</f>
+        <v>0.7033687542392042</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.50288500000000003</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.50288500000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1">
+        <f>(D7+D8+D9)/3</f>
+        <v>0.71459781493075869</v>
+      </c>
+      <c r="E11" s="1">
+        <f>(E7+E8+E9)/3</f>
+        <v>0.72287530214159623</v>
+      </c>
+      <c r="F11" s="1">
+        <f>(F7+F8+F9)/3</f>
+        <v>0.70564451256793281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.55905630516378102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8324FC-0DD2-4B9E-8522-30AD782D09F9}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>1619</v>
+      </c>
+      <c r="B2">
+        <v>1324</v>
+      </c>
+      <c r="C2">
+        <v>1480</v>
+      </c>
+      <c r="D2">
+        <v>1227</v>
+      </c>
+      <c r="L2">
+        <v>1527</v>
+      </c>
+      <c r="M2">
+        <v>1202</v>
+      </c>
+      <c r="N2">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <f>A2-C8</f>
+        <v>1298</v>
+      </c>
+      <c r="C8">
+        <v>321</v>
+      </c>
+      <c r="D8" s="1">
+        <f>B8/(B8+C8)</f>
+        <v>0.80172946263125389</v>
+      </c>
+      <c r="E8" s="1">
+        <f>B8/L2</f>
+        <v>0.85003274394237072</v>
+      </c>
+      <c r="F8" s="1">
+        <f>2*D8*E8/(D8+E8)</f>
+        <v>0.82517482517482521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <f>C2-C9</f>
+        <v>953</v>
+      </c>
+      <c r="C9">
+        <v>527</v>
+      </c>
+      <c r="D9" s="1">
+        <f>B9/(B9+C9)</f>
+        <v>0.64391891891891895</v>
+      </c>
+      <c r="E9" s="1">
+        <f>B9/M2</f>
+        <v>0.79284525790349414</v>
+      </c>
+      <c r="F9" s="1">
+        <f>2*D9*E9/(D9+E9)</f>
+        <v>0.71066368381804634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <f>B2-C10</f>
+        <v>945</v>
+      </c>
+      <c r="C10">
+        <v>379</v>
+      </c>
+      <c r="D10" s="1">
+        <f>B10/(B10+C10)</f>
+        <v>0.71374622356495465</v>
+      </c>
+      <c r="E10" s="1">
+        <f>B10/N2</f>
+        <v>0.55785123966942152</v>
+      </c>
+      <c r="F10" s="1">
+        <f>2*D10*E10/(D10+E10)</f>
+        <v>0.62624254473161045</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <f>(B8+B9+B10)/(B8+B9+B10+C8+C9+C10)</f>
+        <v>0.72258647976486545</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.74856321839080464</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.74856321839080464</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <f>(D8+D9+D10)/3</f>
+        <v>0.7197982017050425</v>
+      </c>
+      <c r="E12" s="1">
+        <f>(E8+E9+E10)/3</f>
+        <v>0.73357641383842875</v>
+      </c>
+      <c r="F12" s="1">
+        <f>(F8+F9+F10)/3</f>
+        <v>0.7206936845748273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.58473773615223901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC16C97-8670-44C8-BD6F-5C240A1DB3DF}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J15:J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1822</v>
+      </c>
+      <c r="B2">
+        <v>809</v>
+      </c>
+      <c r="C2">
+        <v>1738</v>
+      </c>
+      <c r="D2">
+        <v>1082</v>
+      </c>
+      <c r="F2">
+        <v>1527</v>
+      </c>
+      <c r="G2">
+        <v>1202</v>
+      </c>
+      <c r="H2">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <f>A2-C9</f>
+        <v>1424</v>
+      </c>
+      <c r="C9">
+        <v>398</v>
+      </c>
+      <c r="D9" s="1">
+        <f>B9/(B9+C9)</f>
+        <v>0.78155872667398463</v>
+      </c>
+      <c r="E9" s="1">
+        <f>B9/F2</f>
+        <v>0.93254747871643751</v>
+      </c>
+      <c r="F9" s="1">
+        <f>2*D9*E9/(D9+E9)</f>
+        <v>0.8504031054045984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <f>C2-C10</f>
+        <v>1103</v>
+      </c>
+      <c r="C10">
+        <v>635</v>
+      </c>
+      <c r="D10" s="1">
+        <f>B10/(B10+C10)</f>
+        <v>0.63463751438434979</v>
+      </c>
+      <c r="E10" s="1">
+        <f>B10/G2</f>
+        <v>0.91763727121464223</v>
+      </c>
+      <c r="F10" s="1">
+        <f>2*D10*E10/(D10+E10)</f>
+        <v>0.75034013605442162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <f>B2-C11</f>
+        <v>760</v>
+      </c>
+      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1">
+        <f>B11/(B11+C11)</f>
+        <v>0.93943139678615573</v>
+      </c>
+      <c r="E11" s="1">
+        <f>B11/H2</f>
+        <v>0.44864226682408498</v>
+      </c>
+      <c r="F11" s="1">
+        <f>2*D11*E11/(D11+E11)</f>
+        <v>0.60727127447063523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <f>(B9+B10+B11)/(B9+B10+B11+C9+C10+C11)</f>
+        <v>0.75234607461661707</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.56801800000000002</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.56801800000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <f>(D9+D10+D11)/3</f>
+        <v>0.78520921261483012</v>
+      </c>
+      <c r="E13" s="1">
+        <f>(E9+E10+E11)/3</f>
+        <v>0.76627567225172155</v>
+      </c>
+      <c r="F13" s="1">
+        <f>(F9+F10+F11)/3</f>
+        <v>0.73600483864321831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.62281753170675902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>